<commit_message>
Finished Version of EV1
</commit_message>
<xml_diff>
--- a/hardware/EV1 Part Selection.xlsx
+++ b/hardware/EV1 Part Selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finberg\cisco\hactar\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03B6C9E-E12B-4ED1-8CED-57C3367F3907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA61662B-1521-4F33-888A-C0EE2065BAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C8D90A9-3081-44D1-AFD0-F10A6D1B16D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="140">
   <si>
     <t>Component</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Capacitor 22u (X2)</t>
   </si>
   <si>
-    <t>Capacitor 10p (X2)</t>
-  </si>
-  <si>
     <t>Capacitor 10n</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>C1-C2</t>
   </si>
   <si>
-    <t>C3-C4</t>
-  </si>
-  <si>
     <t>C8</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>D2</t>
   </si>
   <si>
-    <t>J1-J2-J6</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
@@ -150,9 +141,6 @@
     <t>J4</t>
   </si>
   <si>
-    <t>J7</t>
-  </si>
-  <si>
     <t>P1</t>
   </si>
   <si>
@@ -210,15 +198,6 @@
     <t>25V 22uF X5R ±20% 0805 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
-    <t>C384748</t>
-  </si>
-  <si>
-    <t>500V 10pF NP0 ±5% 0805 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
-  </si>
-  <si>
-    <t>https://datasheet.lcsc.com/lcsc/1912111437_Walsin-Tech-Corp-0805N100J501CT_C384748.pdf</t>
-  </si>
-  <si>
     <t>50V 1uF X7R ±10% 0805 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
@@ -321,12 +300,6 @@
     <t>SW1-SW2</t>
   </si>
   <si>
-    <t>Capacitor 100n (X5)</t>
-  </si>
-  <si>
-    <t>C5-C11-C12-C13-C14</t>
-  </si>
-  <si>
     <t>Resistor 5.1k (X2)</t>
   </si>
   <si>
@@ -459,16 +432,28 @@
     <t>https://datasheet.lcsc.com/lcsc/2206010216_UNI-ROYAL-Uniroyal-Elec-0805W8F1502T5E_C17475.pdf</t>
   </si>
   <si>
-    <t>C134092</t>
-  </si>
-  <si>
-    <t>Connector_USB:USB_C_Receptacle_Molex_105450-0101</t>
-  </si>
-  <si>
-    <t>1 24 Female Type-C SMD USB Connectors ROHS</t>
-  </si>
-  <si>
-    <t>https://datasheet.lcsc.com/lcsc/1811131824_MOLEX-1054500101_C134092.pdf</t>
+    <t>C4-C5-C11-C12-C13-C14</t>
+  </si>
+  <si>
+    <t>Capacitor 100n (X6)</t>
+  </si>
+  <si>
+    <t>J6-J7-J8</t>
+  </si>
+  <si>
+    <t>J1-J2</t>
+  </si>
+  <si>
+    <t>C165948</t>
+  </si>
+  <si>
+    <t>Connector_USB:USB_C_Receptacle_HRO_TYPE-C-31-M-12</t>
+  </si>
+  <si>
+    <t>5A 1 16 Female Type-C SMD USB Connectors ROHS</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2205251630_Korean-Hroparts-Elec-TYPE-C-31-M-12_C165948.pdf</t>
   </si>
 </sst>
 </file>
@@ -852,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CB574A-5C12-4026-BE97-713F864B6E97}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -863,7 +848,7 @@
     <col min="1" max="1" width="27.26953125" customWidth="1"/>
     <col min="2" max="2" width="21.08984375" customWidth="1"/>
     <col min="3" max="3" width="30.1796875" customWidth="1"/>
-    <col min="4" max="4" width="78.54296875" customWidth="1"/>
+    <col min="4" max="4" width="78.453125" customWidth="1"/>
     <col min="5" max="5" width="14.90625" customWidth="1"/>
     <col min="6" max="6" width="48.08984375" customWidth="1"/>
     <col min="7" max="7" width="12.08984375" customWidth="1"/>
@@ -905,19 +890,19 @@
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G2">
         <v>169368</v>
@@ -926,7 +911,7 @@
         <v>0.01</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
@@ -934,19 +919,19 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G3">
         <v>2832610</v>
@@ -955,210 +940,210 @@
         <v>0.03</v>
       </c>
       <c r="I3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="G4">
-        <v>963</v>
+        <v>964249</v>
       </c>
       <c r="H4" s="3">
-        <v>1.0500000000000001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="G5">
-        <v>964249</v>
+        <v>3877118</v>
       </c>
       <c r="H5" s="3">
         <v>0.01</v>
       </c>
-      <c r="I5" t="s">
-        <v>106</v>
+      <c r="I5" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6">
+        <v>11139435</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
         <v>102</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6">
-        <v>3877118</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="G7">
-        <v>11139435</v>
+        <v>14047</v>
       </c>
       <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0.02</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G8">
-        <v>14047</v>
+        <v>484</v>
       </c>
       <c r="H8" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0.1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>135</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="G9">
-        <v>484</v>
+        <v>317</v>
       </c>
       <c r="H9" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>81</v>
+        <v>0.13</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>112</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
       <c r="G10">
-        <v>317</v>
+        <v>1660</v>
       </c>
       <c r="H10" s="3">
-        <v>0.13</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>114</v>
+        <v>0.19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1166,28 +1151,28 @@
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="G11">
-        <v>1660</v>
+        <v>666</v>
       </c>
       <c r="H11" s="3">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1195,231 +1180,231 @@
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G12">
-        <v>666</v>
+        <v>4490</v>
       </c>
       <c r="H12" s="3">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="I12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G13">
-        <v>4490</v>
+        <v>4563</v>
       </c>
       <c r="H13" s="3">
         <v>0.16</v>
       </c>
       <c r="I13" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="G14">
-        <v>4563</v>
+        <v>44309</v>
       </c>
       <c r="H14" s="3">
-        <v>0.16</v>
+        <v>0.22</v>
       </c>
       <c r="I14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="G15">
-        <v>131932</v>
+        <v>419084</v>
       </c>
       <c r="H15" s="3">
-        <v>0.65</v>
+        <v>0.01</v>
       </c>
       <c r="I15" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G16">
-        <v>419084</v>
+        <v>1220656</v>
       </c>
       <c r="H16" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="I16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17">
+        <v>749086</v>
+      </c>
+      <c r="H17" s="3">
         <v>0.01</v>
       </c>
-      <c r="I16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" t="s">
-        <v>102</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G17">
-        <v>1220656</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0.04</v>
-      </c>
       <c r="I17" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G18">
-        <v>749086</v>
+        <v>2365347</v>
       </c>
       <c r="H18" s="3">
         <v>0.01</v>
       </c>
       <c r="I18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>134</v>
+        <v>61</v>
       </c>
       <c r="G19">
-        <v>2365347</v>
+        <v>1260266</v>
       </c>
       <c r="H19" s="3">
         <v>0.01</v>
       </c>
       <c r="I19" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1427,182 +1412,153 @@
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G20">
-        <v>1260266</v>
+        <v>560155</v>
       </c>
       <c r="H20" s="3">
         <v>0.01</v>
       </c>
       <c r="I20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>102</v>
+        <v>6</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21">
         <v>69</v>
       </c>
-      <c r="G21">
-        <v>560155</v>
-      </c>
       <c r="H21" s="3">
-        <v>0.01</v>
+        <v>0.3</v>
       </c>
       <c r="I21" t="s">
-        <v>140</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G22">
-        <v>69</v>
+        <v>2784</v>
       </c>
       <c r="H22" s="3">
-        <v>0.3</v>
+        <v>11.59</v>
       </c>
       <c r="I22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G23">
-        <v>2784</v>
+        <v>3559</v>
       </c>
       <c r="H23" s="3">
-        <v>11.59</v>
-      </c>
-      <c r="I23" t="s">
-        <v>75</v>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G24">
-        <v>3559</v>
+        <v>1073</v>
       </c>
       <c r="H24" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.81</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25">
-        <v>1073</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0.81</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I8" r:id="rId1" xr:uid="{F7E099EA-D8F5-4874-902F-D765EFE57F57}"/>
-    <hyperlink ref="I24" r:id="rId2" xr:uid="{48496D99-BD3E-4AAE-AE56-63301E6E8DD9}"/>
-    <hyperlink ref="I25" r:id="rId3" xr:uid="{3CFAB30B-4A3B-4703-B0DE-B459A1BFAB70}"/>
-    <hyperlink ref="I6" r:id="rId4" xr:uid="{A70FA5E9-2993-4056-8DDC-B23D54F634E9}"/>
-    <hyperlink ref="I10" r:id="rId5" xr:uid="{6298CBB4-DDF0-45D2-907B-E67C43BB9759}"/>
+    <hyperlink ref="I7" r:id="rId1" xr:uid="{F7E099EA-D8F5-4874-902F-D765EFE57F57}"/>
+    <hyperlink ref="I23" r:id="rId2" xr:uid="{48496D99-BD3E-4AAE-AE56-63301E6E8DD9}"/>
+    <hyperlink ref="I24" r:id="rId3" xr:uid="{3CFAB30B-4A3B-4703-B0DE-B459A1BFAB70}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{A70FA5E9-2993-4056-8DDC-B23D54F634E9}"/>
+    <hyperlink ref="I9" r:id="rId5" xr:uid="{6298CBB4-DDF0-45D2-907B-E67C43BB9759}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>